<commit_message>
Oude map weer terug gezet
</commit_message>
<xml_diff>
--- a/Architecture/Indeling.xlsx
+++ b/Architecture/Indeling.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Zuidkant" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="95">
   <si>
     <t xml:space="preserve">Eigenschappen: </t>
   </si>
   <si>
-    <t>Kleur (r,g,b)</t>
-  </si>
-  <si>
     <t>Kosten met huis 1</t>
   </si>
   <si>
@@ -157,6 +154,159 @@
   </si>
   <si>
     <t>Kosten per huis kopen</t>
+  </si>
+  <si>
+    <t>Gevangenis</t>
+  </si>
+  <si>
+    <t>Oranje</t>
+  </si>
+  <si>
+    <t>3 beurten vast zitten of 50 pm betalen</t>
+  </si>
+  <si>
+    <t>eventueel 50</t>
+  </si>
+  <si>
+    <t>News Sites</t>
+  </si>
+  <si>
+    <t>Fox News</t>
+  </si>
+  <si>
+    <t>violet</t>
+  </si>
+  <si>
+    <t>BBC</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>Illegale bedrijven</t>
+  </si>
+  <si>
+    <t>The Pirate Bay</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Kosten betalen 3 zoekmachines</t>
+  </si>
+  <si>
+    <t>Kosten betalen 4 zoekmachines</t>
+  </si>
+  <si>
+    <t>Muziek streaming</t>
+  </si>
+  <si>
+    <t>Soundcloud</t>
+  </si>
+  <si>
+    <t>oranje</t>
+  </si>
+  <si>
+    <t>Apple Music</t>
+  </si>
+  <si>
+    <t>Spotify</t>
+  </si>
+  <si>
+    <t>Vrij parkeren</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>Wit</t>
+  </si>
+  <si>
+    <t>Geld ontvangen pot</t>
+  </si>
+  <si>
+    <t>Fora</t>
+  </si>
+  <si>
+    <t>4chan</t>
+  </si>
+  <si>
+    <t>Tumblr</t>
+  </si>
+  <si>
+    <t>Reddit</t>
+  </si>
+  <si>
+    <t>rood</t>
+  </si>
+  <si>
+    <t>Kans</t>
+  </si>
+  <si>
+    <t>Geel</t>
+  </si>
+  <si>
+    <t>Bing</t>
+  </si>
+  <si>
+    <t>Webshops</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>eBay</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Popcorn Time</t>
+  </si>
+  <si>
+    <t>Naar de gevangenis</t>
+  </si>
+  <si>
+    <t>Donkerblauw/paars</t>
+  </si>
+  <si>
+    <t>Ga naar de gevangenis (+20 stappen)</t>
+  </si>
+  <si>
+    <t>Facebook</t>
+  </si>
+  <si>
+    <t>Snapchat</t>
+  </si>
+  <si>
+    <t>groen</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>Whatsapp</t>
+  </si>
+  <si>
+    <t>Video Streaming</t>
+  </si>
+  <si>
+    <t>blauw</t>
+  </si>
+  <si>
+    <t>Youtube</t>
+  </si>
+  <si>
+    <t>Netflix</t>
+  </si>
+  <si>
+    <t>Safari</t>
+  </si>
+  <si>
+    <t>4*ogen van de worp</t>
+  </si>
+  <si>
+    <t>10*ogen van de worp</t>
   </si>
 </sst>
 </file>
@@ -592,8 +742,8 @@
   </sheetPr>
   <dimension ref="A1:R105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +751,7 @@
     <col min="1" max="1" width="30.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.140625" style="13" customWidth="1"/>
     <col min="4" max="4" width="15.140625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,120 +764,120 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="11"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="11"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="11"/>
@@ -735,121 +885,157 @@
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B20" s="11">
+        <v>60</v>
+      </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="15"/>
+      <c r="D20" s="15">
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="B22" s="11">
+        <v>2</v>
+      </c>
       <c r="C22" s="5"/>
-      <c r="D22" s="15"/>
+      <c r="D22" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="11">
+        <v>4</v>
+      </c>
       <c r="C23" s="5"/>
-      <c r="D23" s="15"/>
+      <c r="D23" s="15">
+        <v>8</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B24" s="11">
+        <v>50</v>
+      </c>
       <c r="C24" s="5"/>
-      <c r="D24" s="15"/>
+      <c r="D24" s="15">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="B25" s="11">
+        <v>12</v>
+      </c>
       <c r="C25" s="5"/>
-      <c r="D25" s="15"/>
+      <c r="D25" s="15">
+        <v>20</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="B26" s="11">
+        <v>30</v>
+      </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="15"/>
+      <c r="D26" s="15">
+        <v>60</v>
+      </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="B27" s="11">
+        <v>90</v>
+      </c>
       <c r="C27" s="5"/>
-      <c r="D27" s="15"/>
+      <c r="D27" s="15">
+        <v>180</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="B28" s="11">
+        <v>160</v>
+      </c>
       <c r="C28" s="5"/>
-      <c r="D28" s="15"/>
+      <c r="D28" s="15">
+        <v>320</v>
+      </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B29" s="11"/>
+        <v>5</v>
+      </c>
+      <c r="B29" s="11">
+        <v>250</v>
+      </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="15"/>
+      <c r="D29" s="15">
+        <v>450</v>
+      </c>
     </row>
     <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
@@ -862,287 +1048,318 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="R31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="R32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R33" t="s">
         <v>21</v>
-      </c>
-      <c r="R33" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="15"/>
       <c r="R34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R36" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R37" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="R38" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" s="15"/>
+        <v>6</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="R39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="15"/>
+        <v>43</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="R40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41" s="15"/>
+        <v>1</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="R41" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B42" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B43" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B44" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="45" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="16"/>
+        <v>5</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="15"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B54" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="B54" s="15">
+        <v>200</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="15"/>
+        <v>9</v>
+      </c>
+      <c r="B68" s="15">
+        <v>200</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B70" s="15"/>
+        <v>32</v>
+      </c>
+      <c r="B70" s="15">
+        <v>25</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B71" s="15"/>
+        <v>33</v>
+      </c>
+      <c r="B71" s="15">
+        <v>50</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B72" s="15"/>
+        <v>34</v>
+      </c>
+      <c r="B72" s="15">
+        <v>100</v>
+      </c>
     </row>
     <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B73" s="16"/>
+        <v>35</v>
+      </c>
+      <c r="B73" s="16">
+        <v>200</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
@@ -1155,219 +1372,246 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="10"/>
       <c r="E77" s="2"/>
-      <c r="F77" s="3"/>
+      <c r="F77" s="14"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C78" s="5"/>
       <c r="D78" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E78" s="5"/>
       <c r="F78" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E79" s="5"/>
       <c r="F79" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B80" s="11">
+        <v>100</v>
+      </c>
       <c r="C80" s="5"/>
-      <c r="D80" s="11"/>
+      <c r="D80" s="11">
+        <v>100</v>
+      </c>
       <c r="E80" s="5"/>
-      <c r="F80" s="6"/>
+      <c r="F80" s="15">
+        <v>120</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E81" s="5"/>
       <c r="F81" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B82" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="B82" s="11">
+        <v>6</v>
+      </c>
       <c r="C82" s="5"/>
-      <c r="D82" s="11"/>
+      <c r="D82" s="11">
+        <v>6</v>
+      </c>
       <c r="E82" s="5"/>
-      <c r="F82" s="6"/>
+      <c r="F82" s="15">
+        <v>8</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" s="11"/>
+        <v>6</v>
+      </c>
+      <c r="B83" s="11">
+        <v>12</v>
+      </c>
       <c r="C83" s="5"/>
-      <c r="D83" s="11"/>
+      <c r="D83" s="11">
+        <v>12</v>
+      </c>
       <c r="E83" s="5"/>
-      <c r="F83" s="6"/>
+      <c r="F83" s="15">
+        <v>16</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B84" s="11"/>
+        <v>43</v>
+      </c>
+      <c r="B84" s="11">
+        <v>50</v>
+      </c>
       <c r="C84" s="5"/>
-      <c r="D84" s="11"/>
+      <c r="D84" s="11">
+        <v>50</v>
+      </c>
       <c r="E84" s="5"/>
-      <c r="F84" s="6"/>
+      <c r="F84" s="15">
+        <v>50</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B85" s="11"/>
+        <v>1</v>
+      </c>
+      <c r="B85" s="11">
+        <v>30</v>
+      </c>
       <c r="C85" s="5"/>
-      <c r="D85" s="11"/>
+      <c r="D85" s="11">
+        <v>30</v>
+      </c>
       <c r="E85" s="5"/>
-      <c r="F85" s="6"/>
+      <c r="F85" s="15">
+        <v>40</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="B86" s="11">
+        <v>90</v>
+      </c>
       <c r="C86" s="5"/>
-      <c r="D86" s="11"/>
+      <c r="D86" s="11">
+        <v>90</v>
+      </c>
       <c r="E86" s="5"/>
-      <c r="F86" s="6"/>
+      <c r="F86" s="15">
+        <v>100</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="B87" s="11">
+        <v>270</v>
+      </c>
       <c r="C87" s="5"/>
-      <c r="D87" s="11"/>
+      <c r="D87" s="11">
+        <v>270</v>
+      </c>
       <c r="E87" s="5"/>
-      <c r="F87" s="6"/>
+      <c r="F87" s="15">
+        <v>300</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="B88" s="11">
+        <v>400</v>
+      </c>
       <c r="C88" s="5"/>
-      <c r="D88" s="11"/>
+      <c r="D88" s="11">
+        <v>400</v>
+      </c>
       <c r="E88" s="5"/>
-      <c r="F88" s="6"/>
+      <c r="F88" s="15">
+        <v>450</v>
+      </c>
     </row>
     <row r="89" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B89" s="12"/>
+        <v>5</v>
+      </c>
+      <c r="B89" s="12">
+        <v>550</v>
+      </c>
       <c r="C89" s="8"/>
-      <c r="D89" s="12"/>
+      <c r="D89" s="12">
+        <v>550</v>
+      </c>
       <c r="E89" s="8"/>
-      <c r="F89" s="9"/>
-    </row>
-    <row r="92" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="F89" s="16">
+        <v>600</v>
+      </c>
+    </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A93" s="5"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A94" s="5"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="A95" s="5"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="A96" s="5"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>22</v>
-      </c>
+      <c r="A97" s="5"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A98" s="5"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A99" s="5"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A100" s="5"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A101" s="5"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="A102" s="5"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A103" s="5"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="A104" s="5"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1376,38 +1620,2402 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="11">
+        <v>140</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="11">
+        <v>140</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="11">
+        <v>10</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="11">
+        <v>10</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="11">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="11">
+        <v>20</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="11">
+        <v>100</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="11">
+        <v>100</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11">
+        <v>50</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="11">
+        <v>50</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="11">
+        <v>150</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="11">
+        <v>150</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="15">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11">
+        <v>450</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="11">
+        <v>450</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="15">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="11">
+        <v>625</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="11">
+        <v>625</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="15">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="12">
+        <v>750</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="12">
+        <v>750</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="16">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="2"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="14"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="5"/>
+      <c r="D62" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="11">
+        <v>160</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="11">
+        <v>160</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="11">
+        <v>14</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="11">
+        <v>14</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="11">
+        <v>28</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="11">
+        <v>28</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="11">
+        <v>100</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="11">
+        <v>100</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="11">
+        <v>70</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="11">
+        <v>70</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="11">
+        <v>200</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="11">
+        <v>200</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="11">
+        <v>550</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="11">
+        <v>550</v>
+      </c>
+      <c r="E71" s="5"/>
+      <c r="F71" s="15">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="11">
+        <v>750</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="11">
+        <v>750</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="12">
+        <v>950</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="12">
+        <v>950</v>
+      </c>
+      <c r="E73" s="8"/>
+      <c r="F73" s="16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="15"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="15"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="11">
+        <v>220</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="11">
+        <v>220</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="15">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="11">
+        <v>18</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="11">
+        <v>18</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="11">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="11">
+        <v>36</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="11">
+        <v>150</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="11">
+        <v>150</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11">
+        <v>90</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="11">
+        <v>90</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="11">
+        <v>250</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="11">
+        <v>250</v>
+      </c>
+      <c r="E26" s="5"/>
+      <c r="F26" s="15">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="11">
+        <v>700</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="11">
+        <v>700</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="15">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="11">
+        <v>875</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="11">
+        <v>875</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="15">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="12">
+        <v>1050</v>
+      </c>
+      <c r="C29" s="8"/>
+      <c r="D29" s="12">
+        <v>1050</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="16">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="14"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C63" s="5"/>
+      <c r="D63" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C64" s="5"/>
+      <c r="D64" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="5"/>
+      <c r="F64" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="11">
+        <v>260</v>
+      </c>
+      <c r="C65" s="5"/>
+      <c r="D65" s="11">
+        <v>260</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="15">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="5"/>
+      <c r="D66" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="5"/>
+      <c r="F66" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="11">
+        <v>22</v>
+      </c>
+      <c r="C67" s="5"/>
+      <c r="D67" s="11">
+        <v>22</v>
+      </c>
+      <c r="E67" s="5"/>
+      <c r="F67" s="15">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="11">
+        <v>44</v>
+      </c>
+      <c r="C68" s="5"/>
+      <c r="D68" s="11">
+        <v>44</v>
+      </c>
+      <c r="E68" s="5"/>
+      <c r="F68" s="15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="11">
+        <v>150</v>
+      </c>
+      <c r="C69" s="5"/>
+      <c r="D69" s="11">
+        <v>150</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="11">
+        <v>110</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="D70" s="11">
+        <v>110</v>
+      </c>
+      <c r="E70" s="5"/>
+      <c r="F70" s="15">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="11">
+        <v>330</v>
+      </c>
+      <c r="C71" s="5"/>
+      <c r="D71" s="11">
+        <v>330</v>
+      </c>
+      <c r="E71" s="5"/>
+      <c r="F71" s="15">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" s="11">
+        <v>800</v>
+      </c>
+      <c r="C72" s="5"/>
+      <c r="D72" s="11">
+        <v>800</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="15">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" s="11">
+        <v>975</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="11">
+        <v>975</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="15">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="12">
+        <v>1150</v>
+      </c>
+      <c r="C74" s="8"/>
+      <c r="D74" s="12">
+        <v>1150</v>
+      </c>
+      <c r="E74" s="8"/>
+      <c r="F74" s="16">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B80" s="15"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B87" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B89" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="5"/>
+      <c r="F18" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="15"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="15"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="15"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" s="15"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="15"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="15"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="15"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="15"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="16"/>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="15"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="15"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" s="15"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" s="16"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="5"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="15"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C77" s="2"/>
+      <c r="D77" s="14"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="11"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="15"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B82" s="11"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="15"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="11"/>
+      <c r="C83" s="5"/>
+      <c r="D83" s="15"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B84" s="11"/>
+      <c r="C84" s="5"/>
+      <c r="D84" s="15"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="11"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="15"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="11"/>
+      <c r="C86" s="5"/>
+      <c r="D86" s="15"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87" s="11"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="15"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="11"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="15"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="11"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="15"/>
+    </row>
+    <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="7"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="16"/>
+    </row>
+    <row r="93" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" s="15"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B96" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B98" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B99" s="15"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B100" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B101" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B105" s="15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>